<commit_message>
Test scene boat messing, updating project plan
</commit_message>
<xml_diff>
--- a/jumpyStreetProjectPlan.xlsx
+++ b/jumpyStreetProjectPlan.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\__Wake Tech SGD\_2019 Fall Semester\Software Development\Crossy Road 9-25\crossy-road-group-a\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\__Wake Tech SGD\_2019 Fall Semester\Software Development\Crossy Road 10-02\crossy-road-group-a\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="38">
   <si>
     <t>Jumpy Street</t>
   </si>
@@ -53,15 +53,9 @@
     <t>Insert a row above to add more features to the list.</t>
   </si>
   <si>
-    <t>Procedural code</t>
-  </si>
-  <si>
     <t>Movement</t>
   </si>
   <si>
-    <t>Score/High Score</t>
-  </si>
-  <si>
     <t>Death conditions</t>
   </si>
   <si>
@@ -108,6 +102,42 @@
   </si>
   <si>
     <t>Raycasting obstacles</t>
+  </si>
+  <si>
+    <t>Tile generation</t>
+  </si>
+  <si>
+    <t>Random instantiation</t>
+  </si>
+  <si>
+    <t>Character Customization</t>
+  </si>
+  <si>
+    <t>High Score system</t>
+  </si>
+  <si>
+    <t>Update UI with high scores and details</t>
+  </si>
+  <si>
+    <t>Research timed event row (train)</t>
+  </si>
+  <si>
+    <t>Expand tile system to prep instantiation (write water, grass, and car logic)</t>
+  </si>
+  <si>
+    <t>"Max Y" global variable, informs score and camera</t>
+  </si>
+  <si>
+    <t>Setting up player character animations</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>Touch ups</t>
+  </si>
+  <si>
+    <t>Lauren/Andrew</t>
   </si>
 </sst>
 </file>
@@ -541,10 +571,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -566,7 +596,7 @@
     </row>
     <row r="2" spans="1:4" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -612,72 +642,72 @@
     </row>
     <row r="7" spans="1:4" ht="41.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B7" s="10">
         <v>43726</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="41.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B8" s="10">
         <v>43731</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>5</v>
+        <v>18</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="41.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B9" s="10">
         <v>43726</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B10" s="10">
         <v>43726</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B11" s="10">
         <v>43733</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>5</v>
+        <v>18</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -688,141 +718,211 @@
         <v>43733</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" s="13" t="s">
-        <v>5</v>
+        <v>16</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="B13" s="10">
         <v>43733</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B14" s="10">
-        <v>43740</v>
+        <v>43747</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D14" s="14" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D14" s="13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="14" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="B15" s="10">
+        <v>43747</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="14" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="B16" s="10">
+        <v>43747</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="10">
+        <v>43754</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="10"/>
+      <c r="C18" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="9"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="14" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
       <c r="D18" s="14" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B19" s="9"/>
-      <c r="C19" s="9"/>
+        <v>31</v>
+      </c>
+      <c r="B19" s="10"/>
+      <c r="C19" s="9" t="s">
+        <v>18</v>
+      </c>
       <c r="D19" s="14" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
+      <c r="C20" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="D20" s="14" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="5"/>
+    <row r="21" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="5"/>
-    </row>
-    <row r="22" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="5"/>
+      <c r="C21" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>30</v>
+      </c>
       <c r="B22" s="9"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="5"/>
-    </row>
-    <row r="23" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="5"/>
-      <c r="B23" s="9"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="5"/>
-    </row>
-    <row r="24" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="5"/>
-      <c r="B24" s="9"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="5"/>
-    </row>
-    <row r="25" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="5"/>
-      <c r="B25" s="9"/>
-      <c r="C25" s="9"/>
-      <c r="D25" s="5"/>
-    </row>
-    <row r="26" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="5"/>
-      <c r="B26" s="9"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="5"/>
-    </row>
-    <row r="27" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="5"/>
-      <c r="B27" s="9"/>
-      <c r="C27" s="9"/>
-      <c r="D27" s="5"/>
+      <c r="C22" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D26" s="14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D27" s="14" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="28" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="5"/>
@@ -836,28 +936,70 @@
       <c r="C29" s="9"/>
       <c r="D29" s="5"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="5"/>
       <c r="B30" s="9"/>
       <c r="C30" s="9"/>
       <c r="D30" s="5"/>
     </row>
-    <row r="31" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="7" t="s">
+    <row r="31" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="5"/>
+      <c r="B31" s="9"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="5"/>
+    </row>
+    <row r="32" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="5"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="5"/>
+    </row>
+    <row r="33" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="5"/>
+      <c r="B33" s="9"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="5"/>
+    </row>
+    <row r="34" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="5"/>
+      <c r="B34" s="9"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="5"/>
+    </row>
+    <row r="35" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="5"/>
+      <c r="B35" s="9"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="5"/>
+    </row>
+    <row r="36" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="5"/>
+      <c r="B36" s="9"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="5"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="5"/>
+      <c r="B37" s="9"/>
+      <c r="C37" s="9"/>
+      <c r="D37" s="5"/>
+    </row>
+    <row r="38" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
     </row>
   </sheetData>
   <dataConsolidate/>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D20:D29">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D27:D36">
       <formula1>$D$4:$D$6</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Estimated completion date" prompt="Enter the expected due date for the feature." sqref="B3 B10:B29"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Who is in charge of the feature?" prompt="Enter the name of the teammate who is lead for the feature." sqref="C3 C10:C29"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Estimated completion date" prompt="Enter the expected due date for the feature." sqref="B3 B10:B13 B14:B36"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Who is in charge of the feature?" prompt="Enter the name of the teammate who is lead for the feature." sqref="C3 C10:C13 C14:C36"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Status" prompt="Use the dropdown menu to choose: Not implemented, In Progress or Done." sqref="D3"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>